<commit_message>
Removing unnecessary documents for analysis in the scope of this paper
</commit_message>
<xml_diff>
--- a/outputs/descriptives/06_descriptives_mediation_upper_high.xlsx
+++ b/outputs/descriptives/06_descriptives_mediation_upper_high.xlsx
@@ -1,21 +1,98 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCASTRO\Documents\GitHub\Third-Sector-Size-and-Political-Polarization\outputs\descriptives\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B36511-B2E8-4D7B-B4CE-12BA20624757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>vars</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>trimmed</t>
+  </si>
+  <si>
+    <t>mad</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>skew</t>
+  </si>
+  <si>
+    <t>kurtosis</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Country*</t>
+  </si>
+  <si>
+    <t>Third_pillar_size</t>
+  </si>
+  <si>
+    <t>Poli_polarization</t>
+  </si>
+  <si>
+    <t>Trust_ivs</t>
+  </si>
+  <si>
+    <t>Gini_index</t>
+  </si>
+  <si>
+    <t>Facebook_users</t>
+  </si>
+  <si>
+    <t>Loneliness</t>
+  </si>
+  <si>
+    <t>GDP_Most_Recent</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -32,12 +109,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -52,24 +135,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +199,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +233,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +268,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,86 +444,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>vars</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>sd</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>median</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>trimmed</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>mad</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>min</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>max</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>range</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>skew</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>kurtosis</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>se</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Variable</t>
-        </is>
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -449,7 +517,7 @@
         <v>30</v>
       </c>
       <c r="G2">
-        <v>22.239</v>
+        <v>22.239000000000001</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -464,18 +532,16 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>-1.261166331513932</v>
+        <v>-1.2611663315139321</v>
       </c>
       <c r="M2">
-        <v>2.23606797749979</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Country*</t>
-        </is>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -483,45 +549,43 @@
         <v>59</v>
       </c>
       <c r="C3">
-        <v>6.528192645650967</v>
+        <v>6.5281926456509671</v>
       </c>
       <c r="D3">
-        <v>4.288858967386426</v>
+        <v>4.2888589673864264</v>
       </c>
       <c r="E3">
         <v>5.5</v>
       </c>
       <c r="F3">
-        <v>6.183757610807533</v>
+        <v>6.1837576108075334</v>
       </c>
       <c r="G3">
-        <v>4.360248129109782</v>
+        <v>4.3602481291097819</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="J3">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="K3">
-        <v>0.7074694214613905</v>
+        <v>0.70746942146139047</v>
       </c>
       <c r="L3">
-        <v>-0.519056195436562</v>
+        <v>-0.51905619543656201</v>
       </c>
       <c r="M3">
-        <v>0.5583618783143797</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Third_pillar_size</t>
-        </is>
+        <v>0.55836187831437967</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -529,45 +593,43 @@
         <v>59</v>
       </c>
       <c r="C4">
-        <v>60.25338983050847</v>
+        <v>60.253389830508468</v>
       </c>
       <c r="D4">
-        <v>23.04880198174491</v>
+        <v>23.048801981744909</v>
       </c>
       <c r="E4">
         <v>62.5</v>
       </c>
       <c r="F4">
-        <v>61.07448979591837</v>
+        <v>61.074489795918367</v>
       </c>
       <c r="G4">
-        <v>23.832795</v>
+        <v>23.832795000000001</v>
       </c>
       <c r="H4">
-        <v>8.325000000000001</v>
+        <v>8.3250000000000011</v>
       </c>
       <c r="I4">
         <v>100</v>
       </c>
       <c r="J4">
-        <v>91.675</v>
+        <v>91.674999999999997</v>
       </c>
       <c r="K4">
         <v>-0.3579715761808806</v>
       </c>
       <c r="L4">
-        <v>-0.7590439419571204</v>
+        <v>-0.75904394195712044</v>
       </c>
       <c r="M4">
-        <v>3.000698429416024</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Poli_polarization</t>
-        </is>
+        <v>3.0006984294160239</v>
+      </c>
+      <c r="N4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -575,45 +637,43 @@
         <v>59</v>
       </c>
       <c r="C5">
-        <v>27.415884</v>
+        <v>27.415883999999998</v>
       </c>
       <c r="D5">
-        <v>17.47919420816987</v>
+        <v>17.479194208169869</v>
       </c>
       <c r="E5">
         <v>23.28115</v>
       </c>
       <c r="F5">
-        <v>25.67693414285714</v>
+        <v>25.676934142857139</v>
       </c>
       <c r="G5">
-        <v>14.390026644</v>
+        <v>14.390026644000001</v>
       </c>
       <c r="H5">
         <v>2.77237</v>
       </c>
       <c r="I5">
-        <v>73.86647000000001</v>
+        <v>73.866470000000007</v>
       </c>
       <c r="J5">
-        <v>71.09410000000001</v>
+        <v>71.094100000000012</v>
       </c>
       <c r="K5">
-        <v>0.9140455465612107</v>
+        <v>0.91404554656121073</v>
       </c>
       <c r="L5">
-        <v>0.2126408072815691</v>
+        <v>0.21264080728156909</v>
       </c>
       <c r="M5">
-        <v>2.27559725878396</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Trust_ivs</t>
-        </is>
+        <v>2.2755972587839599</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -621,10 +681,10 @@
         <v>59</v>
       </c>
       <c r="C6">
-        <v>34.60847457627118</v>
+        <v>34.608474576271178</v>
       </c>
       <c r="D6">
-        <v>7.583791430448848</v>
+        <v>7.5837914304488478</v>
       </c>
       <c r="E6">
         <v>33.5</v>
@@ -645,67 +705,63 @@
         <v>38.9</v>
       </c>
       <c r="K6">
-        <v>1.374475100864973</v>
+        <v>1.3744751008649729</v>
       </c>
       <c r="L6">
-        <v>2.397929524035472</v>
+        <v>2.3979295240354719</v>
       </c>
       <c r="M6">
         <v>0.98732554743584</v>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Gini_index</t>
-        </is>
+      <c r="N6" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7">
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>59</v>
       </c>
-      <c r="C7">
-        <v>70068.47149694794</v>
-      </c>
-      <c r="D7">
-        <v>12048.96245386898</v>
-      </c>
-      <c r="E7">
-        <v>70198.82140787532</v>
-      </c>
-      <c r="F7">
-        <v>70190.10089133575</v>
-      </c>
-      <c r="G7">
-        <v>10870.16492867057</v>
-      </c>
-      <c r="H7">
-        <v>43131.03276276811</v>
-      </c>
-      <c r="I7">
-        <v>98730.47124702754</v>
-      </c>
-      <c r="J7">
-        <v>55599.43848425943</v>
-      </c>
-      <c r="K7">
-        <v>-0.04611152244727727</v>
-      </c>
-      <c r="L7">
-        <v>-0.2100513136573166</v>
-      </c>
-      <c r="M7">
-        <v>1568.641300318038</v>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>Facebook_users</t>
-        </is>
+      <c r="C7" s="2">
+        <v>73224.338516918127</v>
+      </c>
+      <c r="D7" s="2">
+        <v>15978.13830678619</v>
+      </c>
+      <c r="E7" s="2">
+        <v>73724.614872807841</v>
+      </c>
+      <c r="F7" s="2">
+        <v>74250.786328817732</v>
+      </c>
+      <c r="G7" s="2">
+        <v>13831.25331232013</v>
+      </c>
+      <c r="H7" s="2">
+        <v>415.00349858636088</v>
+      </c>
+      <c r="I7" s="2">
+        <v>102446.0482241939</v>
+      </c>
+      <c r="J7" s="2">
+        <v>102031.0447256076</v>
+      </c>
+      <c r="K7" s="2">
+        <v>-1.5081962647096321</v>
+      </c>
+      <c r="L7" s="2">
+        <v>5.3471559240627222</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2080.1764256614788</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -713,45 +769,43 @@
         <v>59</v>
       </c>
       <c r="C8">
-        <v>24.94339110530509</v>
+        <v>24.943391105305089</v>
       </c>
       <c r="D8">
-        <v>10.98835279465595</v>
+        <v>10.988352794655951</v>
       </c>
       <c r="E8">
         <v>25</v>
       </c>
       <c r="F8">
-        <v>24.93408234734694</v>
+        <v>24.934082347346941</v>
       </c>
       <c r="G8">
         <v>12.897636576594</v>
       </c>
       <c r="H8">
-        <v>4.326958785</v>
+        <v>4.3269587850000004</v>
       </c>
       <c r="I8">
         <v>45.8</v>
       </c>
       <c r="J8">
-        <v>41.47304121499999</v>
+        <v>41.473041214999988</v>
       </c>
       <c r="K8">
-        <v>-0.04460820252678459</v>
+        <v>-4.4608202526784588E-2</v>
       </c>
       <c r="L8">
-        <v>-0.9823682821932205</v>
+        <v>-0.98236828219322048</v>
       </c>
       <c r="M8">
         <v>1.43056168380935</v>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>Loneliness</t>
-        </is>
+      <c r="N8" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -762,39 +816,37 @@
         <v>1012275080832.47</v>
       </c>
       <c r="D9">
-        <v>2805061699960.257</v>
+        <v>2805061699960.2568</v>
       </c>
       <c r="E9">
-        <v>281423471715.402</v>
+        <v>281423471715.40198</v>
       </c>
       <c r="F9">
         <v>504739259563.5191</v>
       </c>
       <c r="G9">
-        <v>348278369857.9423</v>
+        <v>348278369857.94232</v>
       </c>
       <c r="H9">
-        <v>4869340027.24234</v>
+        <v>4869340027.2423401</v>
       </c>
       <c r="I9">
         <v>20926835051000</v>
       </c>
       <c r="J9">
-        <v>20921965710972.76</v>
+        <v>20921965710972.762</v>
       </c>
       <c r="K9">
-        <v>6.105819043367637</v>
+        <v>6.1058190433676369</v>
       </c>
       <c r="L9">
-        <v>40.12892085805341</v>
+        <v>40.128920858053412</v>
       </c>
       <c r="M9">
-        <v>365187927951.8444</v>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>GDP_Most_Recent</t>
-        </is>
+        <v>365187927951.84442</v>
+      </c>
+      <c r="N9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>